<commit_message>
Sample Track Report V2.0
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempSampleTrack.xlsx
+++ b/DKS-API/Resources/Template/TempSampleTrack.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>SampleNo</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -125,6 +125,22 @@
   </si>
   <si>
     <t>&amp;=result.OverDays</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeptName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TransferName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.DeptName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.TransferName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -517,11 +533,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -537,12 +553,13 @@
     <col min="9" max="9" width="14.625" style="7" customWidth="1"/>
     <col min="10" max="10" width="12.875" style="4" customWidth="1"/>
     <col min="11" max="11" width="19.375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="12.875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="19.375" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="4"/>
+    <col min="12" max="13" width="12.875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="19.375" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,10 +597,16 @@
         <v>22</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -621,11 +644,17 @@
         <v>23</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1"/>
+  <autoFilter ref="A1:O1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>